<commit_message>
Made changes to the starter analysis
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05D633ED-4006-4322-B364-4CEFDB16E0D7}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="945" windowWidth="48840" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Codebook" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Height</t>
   </si>
@@ -72,12 +83,27 @@
   </si>
   <si>
     <t>identified gender (male/female/other)</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Individual Income in usd</t>
+  </si>
+  <si>
+    <t>Body mass index in kg/m2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +443,14 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>180</v>
       </c>
@@ -427,8 +460,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>70000</v>
+      </c>
+      <c r="E2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>175</v>
       </c>
@@ -438,8 +477,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>80000</v>
+      </c>
+      <c r="E3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -449,8 +494,14 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>90000</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
@@ -460,8 +511,14 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>95000</v>
+      </c>
+      <c r="E5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>192</v>
       </c>
@@ -471,8 +528,14 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>75000</v>
+      </c>
+      <c r="E6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -482,8 +545,14 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>85000</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>156</v>
       </c>
@@ -493,8 +562,14 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>89000</v>
+      </c>
+      <c r="E8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>166</v>
       </c>
@@ -504,8 +579,14 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>85000</v>
+      </c>
+      <c r="E9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>155</v>
       </c>
@@ -515,8 +596,14 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>92000</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>145</v>
       </c>
@@ -526,16 +613,28 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>78000</v>
+      </c>
+      <c r="E11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>165</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>110000</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>133</v>
       </c>
@@ -545,8 +644,14 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>166</v>
       </c>
@@ -556,8 +661,14 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>154</v>
       </c>
@@ -566,6 +677,13 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>96000</v>
+      </c>
+      <c r="E15">
+        <f>ROUND(B15/((A15/100)^2),0)</f>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -575,16 +693,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -632,6 +750,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>